<commit_message>
Replaced obsolete RED LED.
</commit_message>
<xml_diff>
--- a/Electronics/v7.3/FED3_v7.3 BOM.xlsx
+++ b/Electronics/v7.3/FED3_v7.3 BOM.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filip\Documents\GitHub\open-ephys\FED3\Electronics\v7.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32D6BD5E-F319-4984-8716-7DEA3D2DBCA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35B6915-D8F5-4B7C-A2F6-58F5E273DACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A5D68449-08D0-40BF-AC30-C7AAF2663176}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A5D68449-08D0-40BF-AC30-C7AAF2663176}"/>
   </bookViews>
   <sheets>
     <sheet name="FED3_v7.3 BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -190,12 +203,6 @@
     <t>RED</t>
   </si>
   <si>
-    <t>OEPS030006</t>
-  </si>
-  <si>
-    <t>5975004407F</t>
-  </si>
-  <si>
     <t>D2</t>
   </si>
   <si>
@@ -514,9 +521,6 @@
     <t>LTST-C191KGKT</t>
   </si>
   <si>
-    <t>DIODE: LED 0603 Red 635nm 20mA [5975004407F] [0603]</t>
-  </si>
-  <si>
     <t>DIODE: Schottky 20V 1A [SM5817PL-TP] [SOD-123FL]</t>
   </si>
   <si>
@@ -620,6 +624,15 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>OEPS030038</t>
+  </si>
+  <si>
+    <t>VFHR1116P-4C82A-TR</t>
+  </si>
+  <si>
+    <t>DIODE: LED 0603 Red 635nm 20mA [VFHR1116P-4C82A-TR] [0603]</t>
   </si>
 </sst>
 </file>
@@ -1491,7 +1504,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,7 +1520,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1525,10 +1538,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1558,7 +1571,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -1570,7 +1583,7 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1594,10 +1607,10 @@
         <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1621,10 +1634,10 @@
         <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1648,10 +1661,10 @@
         <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1675,10 +1688,10 @@
         <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1702,10 +1715,10 @@
         <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1729,10 +1742,10 @@
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1756,10 +1769,10 @@
         <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1783,10 +1796,10 @@
         <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H11" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1810,10 +1823,10 @@
         <v>8</v>
       </c>
       <c r="G12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1837,10 +1850,10 @@
         <v>8</v>
       </c>
       <c r="G13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1858,16 +1871,16 @@
         <v>52</v>
       </c>
       <c r="E14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F14" t="s">
         <v>53</v>
       </c>
       <c r="G14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1882,19 +1895,19 @@
         <v>55</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>197</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>198</v>
       </c>
       <c r="F15" t="s">
         <v>53</v>
       </c>
       <c r="G15" t="s">
-        <v>164</v>
+        <v>199</v>
       </c>
       <c r="H15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1903,25 +1916,25 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
         <v>58</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>59</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16" t="s">
         <v>60</v>
       </c>
-      <c r="E16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" t="s">
-        <v>62</v>
-      </c>
       <c r="G16" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H16" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1930,25 +1943,25 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" t="s">
         <v>63</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" t="s">
         <v>64</v>
       </c>
-      <c r="D17" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" t="s">
-        <v>66</v>
-      </c>
       <c r="G17" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1957,25 +1970,25 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" t="s">
         <v>67</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
         <v>68</v>
       </c>
-      <c r="D18" t="s">
+      <c r="F18" t="s">
         <v>69</v>
       </c>
-      <c r="E18" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" t="s">
-        <v>71</v>
-      </c>
       <c r="G18" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1984,25 +1997,25 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" t="s">
         <v>72</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E19" t="s">
         <v>73</v>
       </c>
-      <c r="D19" t="s">
+      <c r="F19" t="s">
         <v>74</v>
       </c>
-      <c r="E19" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" t="s">
-        <v>76</v>
-      </c>
       <c r="G19" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H19" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -2011,25 +2024,25 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>75</v>
+      </c>
+      <c r="C20" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" t="s">
         <v>77</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F20" t="s">
         <v>78</v>
       </c>
-      <c r="D20" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="F20" t="s">
-        <v>80</v>
-      </c>
       <c r="G20" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="H20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2038,25 +2051,25 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" t="s">
         <v>81</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
         <v>82</v>
       </c>
-      <c r="D21" t="s">
+      <c r="F21" t="s">
         <v>83</v>
       </c>
-      <c r="E21" t="s">
-        <v>84</v>
-      </c>
-      <c r="F21" t="s">
-        <v>85</v>
-      </c>
       <c r="G21" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="H21" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2065,25 +2078,25 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" t="s">
         <v>86</v>
       </c>
-      <c r="C22" t="s">
+      <c r="E22" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F22" t="s">
         <v>87</v>
       </c>
-      <c r="D22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="F22" t="s">
-        <v>89</v>
-      </c>
       <c r="G22" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -2092,25 +2105,25 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" t="s">
         <v>90</v>
       </c>
-      <c r="C23" t="s">
+      <c r="E23" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F23" t="s">
         <v>91</v>
       </c>
-      <c r="D23" t="s">
-        <v>92</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="F23" t="s">
-        <v>93</v>
-      </c>
       <c r="G23" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="H23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2119,25 +2132,25 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" t="s">
         <v>94</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
         <v>95</v>
       </c>
-      <c r="D24" t="s">
+      <c r="F24" t="s">
         <v>96</v>
       </c>
-      <c r="E24" t="s">
-        <v>97</v>
-      </c>
-      <c r="F24" t="s">
-        <v>98</v>
-      </c>
       <c r="G24" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="H24" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -2146,25 +2159,25 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D25" t="s">
         <v>99</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E25" t="s">
         <v>100</v>
       </c>
-      <c r="D25" t="s">
+      <c r="F25" t="s">
         <v>101</v>
       </c>
-      <c r="E25" t="s">
-        <v>102</v>
-      </c>
-      <c r="F25" t="s">
-        <v>103</v>
-      </c>
       <c r="G25" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="H25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2173,25 +2186,25 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26" t="s">
         <v>104</v>
       </c>
-      <c r="C26" t="s">
+      <c r="E26" t="s">
+        <v>175</v>
+      </c>
+      <c r="F26" t="s">
         <v>105</v>
       </c>
-      <c r="D26" t="s">
-        <v>106</v>
-      </c>
-      <c r="E26" t="s">
-        <v>178</v>
-      </c>
-      <c r="F26" t="s">
-        <v>107</v>
-      </c>
       <c r="G26" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -2200,25 +2213,25 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" t="s">
         <v>108</v>
       </c>
-      <c r="C27" t="s">
-        <v>109</v>
-      </c>
-      <c r="D27" t="s">
-        <v>110</v>
-      </c>
       <c r="E27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G27" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H27" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -2227,25 +2240,25 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" t="s">
         <v>111</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E28" t="s">
+        <v>178</v>
+      </c>
+      <c r="F28" t="s">
         <v>112</v>
       </c>
-      <c r="D28" t="s">
-        <v>113</v>
-      </c>
-      <c r="E28" t="s">
-        <v>181</v>
-      </c>
-      <c r="F28" t="s">
-        <v>114</v>
-      </c>
       <c r="G28" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H28" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2254,25 +2267,25 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" t="s">
         <v>115</v>
       </c>
-      <c r="C29" t="s">
+      <c r="E29" t="s">
         <v>116</v>
       </c>
-      <c r="D29" t="s">
+      <c r="F29" t="s">
         <v>117</v>
       </c>
-      <c r="E29" t="s">
-        <v>118</v>
-      </c>
-      <c r="F29" t="s">
-        <v>119</v>
-      </c>
       <c r="G29" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="H29" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -2281,25 +2294,25 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C30" t="s">
+        <v>119</v>
+      </c>
+      <c r="D30" t="s">
         <v>120</v>
       </c>
-      <c r="C30" t="s">
-        <v>121</v>
-      </c>
-      <c r="D30" t="s">
-        <v>122</v>
-      </c>
       <c r="E30" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G30" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H30" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -2308,25 +2321,25 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" t="s">
         <v>123</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
         <v>124</v>
       </c>
-      <c r="D31" t="s">
+      <c r="F31" t="s">
         <v>125</v>
       </c>
-      <c r="E31" t="s">
-        <v>126</v>
-      </c>
-      <c r="F31" t="s">
-        <v>127</v>
-      </c>
       <c r="G31" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H31" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -2335,25 +2348,25 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" t="s">
+        <v>127</v>
+      </c>
+      <c r="D32" t="s">
         <v>128</v>
       </c>
-      <c r="C32" t="s">
+      <c r="E32" t="s">
+        <v>183</v>
+      </c>
+      <c r="F32" t="s">
         <v>129</v>
       </c>
-      <c r="D32" t="s">
-        <v>130</v>
-      </c>
-      <c r="E32" t="s">
-        <v>186</v>
-      </c>
-      <c r="F32" t="s">
-        <v>131</v>
-      </c>
       <c r="G32" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H32" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2362,25 +2375,25 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
+        <v>130</v>
+      </c>
+      <c r="C33" t="s">
+        <v>131</v>
+      </c>
+      <c r="D33" t="s">
         <v>132</v>
       </c>
-      <c r="C33" t="s">
+      <c r="E33" t="s">
         <v>133</v>
       </c>
-      <c r="D33" t="s">
+      <c r="F33" t="s">
         <v>134</v>
       </c>
-      <c r="E33" t="s">
-        <v>135</v>
-      </c>
-      <c r="F33" t="s">
-        <v>136</v>
-      </c>
       <c r="G33" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="H33" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2389,25 +2402,25 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" t="s">
+        <v>136</v>
+      </c>
+      <c r="D34" t="s">
         <v>137</v>
       </c>
-      <c r="C34" t="s">
+      <c r="E34" t="s">
         <v>138</v>
       </c>
-      <c r="D34" t="s">
+      <c r="F34" t="s">
         <v>139</v>
       </c>
-      <c r="E34" t="s">
-        <v>140</v>
-      </c>
-      <c r="F34" t="s">
-        <v>141</v>
-      </c>
       <c r="G34" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H34" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -2416,25 +2429,25 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
+        <v>140</v>
+      </c>
+      <c r="C35" t="s">
+        <v>141</v>
+      </c>
+      <c r="D35" t="s">
         <v>142</v>
       </c>
-      <c r="C35" t="s">
+      <c r="E35" t="s">
         <v>143</v>
       </c>
-      <c r="D35" t="s">
+      <c r="F35" t="s">
         <v>144</v>
       </c>
-      <c r="E35" t="s">
-        <v>145</v>
-      </c>
-      <c r="F35" t="s">
-        <v>146</v>
-      </c>
       <c r="G35" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H35" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -2443,25 +2456,25 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
+        <v>145</v>
+      </c>
+      <c r="C36" t="s">
+        <v>146</v>
+      </c>
+      <c r="D36" t="s">
         <v>147</v>
       </c>
-      <c r="C36" t="s">
+      <c r="E36" t="s">
+        <v>188</v>
+      </c>
+      <c r="F36" t="s">
         <v>148</v>
       </c>
-      <c r="D36" t="s">
-        <v>149</v>
-      </c>
-      <c r="E36" t="s">
-        <v>191</v>
-      </c>
-      <c r="F36" t="s">
-        <v>150</v>
-      </c>
       <c r="G36" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="H36" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>